<commit_message>
Added screws and t-nuts to list
</commit_message>
<xml_diff>
--- a/00-Docs/Rocker-Bogie-Sheets/Materials.xlsx
+++ b/00-Docs/Rocker-Bogie-Sheets/Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw-Material" sheetId="1" r:id="rId1"/>
+    <sheet name="Screws T-Nuts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Materials</t>
   </si>
@@ -94,12 +95,60 @@
   <si>
     <t>Wheel Connector 30mm Part 1
 Wheel Connector 30mm Part 2</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Zylinderschraube DIN 7984 M5 x 12</t>
+  </si>
+  <si>
+    <t>Zylinderschraube DIN 7984 M6 x 12</t>
+  </si>
+  <si>
+    <t>Zylinderschraube DIN 7984 M6 x 16</t>
+  </si>
+  <si>
+    <t>Senkschraube ISO 10642 M6 x 16</t>
+  </si>
+  <si>
+    <t>Zylinderschraube DIN 7984 M8 x 12</t>
+  </si>
+  <si>
+    <t>Zylinderschraube DIN 7984 M5 x 10</t>
+  </si>
+  <si>
+    <t>Nutenstein N8 - M8</t>
+  </si>
+  <si>
+    <t>Nutenstein N8 - M6</t>
+  </si>
+  <si>
+    <t>Nutenstein N6 - M5</t>
+  </si>
+  <si>
+    <t>T-Nut</t>
+  </si>
+  <si>
+    <t>Pkg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +202,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -166,10 +224,25 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,286 +570,286 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="8">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="4">
         <v>65</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>100</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="4">
         <v>100</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="4">
         <v>30</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <v>105</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="4">
         <v>2</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="8">
         <v>40</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="8">
         <v>2</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="8">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4">
         <v>50</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
         <v>105</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="4">
         <v>2</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="8">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="4">
         <v>85</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
         <v>30</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="4">
         <v>2</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="8">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4">
         <v>110</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>60</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="4">
         <v>15</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <v>4</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="4">
         <v>29.5</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>60</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="4">
         <v>25</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <v>4</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="8" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>40</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="4">
         <v>20</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="4">
         <v>4</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>50</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="4">
         <v>30</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>4</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -784,9 +857,9 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -794,9 +867,9 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -804,9 +877,9 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -814,9 +887,9 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -824,9 +897,9 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -849,6 +922,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A1:I2"/>
@@ -865,15 +945,216 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="15">
+        <v>20</v>
+      </c>
+      <c r="E3" s="16">
+        <v>6.45</v>
+      </c>
+      <c r="F3" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15">
+        <v>32</v>
+      </c>
+      <c r="E4" s="16">
+        <v>6.18</v>
+      </c>
+      <c r="F4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="15">
+        <v>8</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5.35</v>
+      </c>
+      <c r="F5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="15">
+        <v>8</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5.39</v>
+      </c>
+      <c r="F6" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15">
+        <v>12</v>
+      </c>
+      <c r="E7" s="16">
+        <v>7.29</v>
+      </c>
+      <c r="F7" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
+      <c r="E8" s="16">
+        <v>3.37</v>
+      </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14">
+        <v>16</v>
+      </c>
+      <c r="E10" s="16">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14">
+        <v>8</v>
+      </c>
+      <c r="E11" s="16">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F11" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14">
+        <v>12</v>
+      </c>
+      <c r="E12" s="16">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>